<commit_message>
Push - red path actions added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\SOSR_PNRCancellation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAB2BF2-08FB-40E5-B420-3BD2BB85D849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB263AC-81E5-4534-AAF4-603D9C232B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,24 @@
   </si>
   <si>
     <t>UAT - AUTOMATION / BOOKING ATTEMPTED TO BE CANCELLED, HOWEVER THE HOTEL FAILED TO CANCEL.</t>
+  </si>
+  <si>
+    <t>strHotelCancelledRemarkText</t>
+  </si>
+  <si>
+    <t>UAT - AUTOMATION / BOOKING CANCELLED, HOWEVER AN ERROR MESSAGE HAS BEEN RECEIVED. THE AUTOMATION HAS CHECKED THERE’S NO LIVE HOTEL COMPONENTS IN THE ITINERARY</t>
+  </si>
+  <si>
+    <t>Remark text when cancellation fails and hotel component is not live</t>
+  </si>
+  <si>
+    <t>strRedPathRemarkText</t>
+  </si>
+  <si>
+    <t>Remark text, whenever a cancellation needs to be done directly in FLY</t>
+  </si>
+  <si>
+    <t>UAT - AUTOMATION / BOOKING ATTEMPTED TO BE CANCELLED, HOWEVER RECEIVED ERROR MESSAGE AND UNABLE TO COMMIT. THE GROUND PASSED TO WNS TO PROCESS</t>
   </si>
 </sst>
 </file>
@@ -1723,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1960,8 +1978,28 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2937,8 +2975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3125,7 +3163,20 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
push before maintaining vm
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\SOSR_PNRCancellation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D4A9A-00E0-4FC8-A82D-9663854452AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA602E5-EBC0-405A-8CBB-1F11098E9D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -395,9 +395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -435,7 +435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -541,7 +541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1777,7 +1777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>